<commit_message>
update: Subindo a primeira e a segunda página do Projeto - Desigualdade na Educação Brasileira.
</commit_message>
<xml_diff>
--- a/Dados-limpos.xlsx
+++ b/Dados-limpos.xlsx
@@ -180,7 +180,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +191,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -227,13 +233,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -638,7 +644,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -703,7 +709,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -768,7 +774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -833,7 +839,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -898,7 +904,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -963,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1353,7 +1359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1678,7 +1684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
@@ -1873,7 +1879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1938,7 +1944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>

</xml_diff>